<commit_message>
applying the food patchup to other sectors (was only applied to electricity production sectors so far)
</commit_message>
<xml_diff>
--- a/src/Data/Exiobase_patchwork.xlsx
+++ b/src/Data/Exiobase_patchwork.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECCE847-9360-46BD-A6D1-70894A328F2B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCF53E4-D8C3-4581-9C67-744FA2A9C96A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22260" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22212" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,7 +484,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -590,65 +590,65 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1</v>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
       </c>
       <c r="I2" s="2">
         <v>1</v>
       </c>
-      <c r="J2" s="2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2">
-        <v>1</v>
-      </c>
-      <c r="O2" s="2">
-        <v>1</v>
-      </c>
-      <c r="P2" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>1</v>
-      </c>
-      <c r="R2" s="2">
-        <v>1</v>
-      </c>
-      <c r="S2" s="2">
-        <v>1</v>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
       </c>
       <c r="T2" s="1">
         <v>0</v>
       </c>
-      <c r="U2" s="2">
-        <v>1</v>
-      </c>
-      <c r="V2" s="2">
-        <v>1</v>
-      </c>
-      <c r="W2" s="2">
-        <v>1</v>
-      </c>
-      <c r="X2" s="2">
-        <v>1</v>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -664,65 +664,65 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
       </c>
       <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1</v>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
       </c>
       <c r="L3" s="2">
         <v>1</v>
       </c>
-      <c r="M3" s="2">
-        <v>1</v>
-      </c>
-      <c r="N3" s="2">
-        <v>1</v>
-      </c>
-      <c r="O3" s="2">
-        <v>1</v>
-      </c>
-      <c r="P3" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>1</v>
-      </c>
-      <c r="R3" s="2">
-        <v>1</v>
-      </c>
-      <c r="S3" s="2">
-        <v>1</v>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
       </c>
       <c r="T3" s="1">
         <v>0</v>
       </c>
-      <c r="U3" s="2">
-        <v>1</v>
-      </c>
-      <c r="V3" s="2">
-        <v>1</v>
-      </c>
-      <c r="W3" s="2">
-        <v>1</v>
-      </c>
-      <c r="X3" s="2">
-        <v>1</v>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
@@ -1099,74 +1099,74 @@
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1</v>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
       </c>
       <c r="I9" s="2">
         <v>1</v>
       </c>
-      <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1</v>
-      </c>
-      <c r="L9" s="2">
-        <v>1</v>
-      </c>
-      <c r="M9" s="2">
-        <v>1</v>
-      </c>
-      <c r="N9" s="2">
-        <v>1</v>
-      </c>
-      <c r="O9" s="2">
-        <v>1</v>
-      </c>
-      <c r="P9" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>1</v>
-      </c>
-      <c r="R9" s="2">
-        <v>1</v>
-      </c>
-      <c r="S9" s="2">
-        <v>1</v>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
       </c>
       <c r="T9" s="1">
         <v>0</v>
       </c>
-      <c r="U9" s="2">
-        <v>1</v>
-      </c>
-      <c r="V9" s="2">
-        <v>1</v>
-      </c>
-      <c r="W9" s="2">
-        <v>1</v>
-      </c>
-      <c r="X9" s="2">
-        <v>1</v>
+      <c r="U9" s="1">
+        <v>0</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0</v>
+      </c>
+      <c r="X9" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">

</xml_diff>